<commit_message>
updated README.md for object orientated approach
</commit_message>
<xml_diff>
--- a/csv_cleaned/cleaned_dataframe.xlsx
+++ b/csv_cleaned/cleaned_dataframe.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bra0008c/Documents/SourceCode/csv_costanalyser/csv_cleaned/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79ADDA10-274C-7643-9937-188BF3E39580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="24080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -373,8 +367,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,14 +431,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -491,7 +477,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -523,27 +509,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -575,24 +543,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -768,46 +718,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="225.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -896,7 +814,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -982,7 +900,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1068,7 +986,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1154,7 +1072,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1240,7 +1158,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1326,7 +1244,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1412,7 +1330,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1498,7 +1416,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1584,7 +1502,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1604,7 +1522,7 @@
         <v>53</v>
       </c>
       <c r="G10">
-        <v>-2.2799999999999998</v>
+        <v>-2.28</v>
       </c>
       <c r="H10" t="s">
         <v>63</v>
@@ -1670,7 +1588,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1690,7 +1608,7 @@
         <v>53</v>
       </c>
       <c r="G11">
-        <v>-9.8000000000000007</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="H11" t="s">
         <v>63</v>
@@ -1756,7 +1674,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1842,7 +1760,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1928,7 +1846,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -2014,7 +1932,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2100,7 +2018,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2186,7 +2104,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2272,7 +2190,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2358,7 +2276,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -2444,7 +2362,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2530,7 +2448,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -2616,7 +2534,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2702,7 +2620,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -2791,7 +2709,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2877,7 +2795,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -2960,7 +2878,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -3046,7 +2964,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29">
       <c r="A27" t="s">
         <v>29</v>
       </c>

</xml_diff>